<commit_message>
new Order And OrderRegistration Added
</commit_message>
<xml_diff>
--- a/Database Overview Diagram/FinalDatabase Overview.xlsx
+++ b/Database Overview Diagram/FinalDatabase Overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prashnat\Desktop\Project\Database Overview Diagram\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CDAC 2023 Knowit Tushar\Git PROJECT\CDac_Project\Database Overview Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195A2F7C-2C56-40A3-9A2F-4C84AAF94DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107A56F2-B8F8-43D3-AC6A-E24D8527D668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1392" yWindow="1716" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,6 +342,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -357,7 +358,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B93" zoomScale="113" zoomScaleNormal="203" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I107" sqref="I107:I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,46 +668,46 @@
   </cols>
   <sheetData>
     <row r="3" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
     </row>
     <row r="4" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
     </row>
     <row r="5" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
     </row>
     <row r="7" spans="5:15" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H7" s="5"/>
@@ -720,12 +720,12 @@
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="5:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="9"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -801,12 +801,12 @@
       <c r="O13" s="5"/>
     </row>
     <row r="14" spans="5:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -993,16 +993,16 @@
       </c>
     </row>
     <row r="27" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G27" s="11">
+      <c r="G27" s="6">
         <v>12</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="H27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1013,12 +1013,12 @@
       <c r="J28" s="4"/>
     </row>
     <row r="31" spans="7:13" x14ac:dyDescent="0.3">
-      <c r="G31" s="6" t="s">
+      <c r="G31" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="9"/>
     </row>
     <row r="32" spans="7:13" x14ac:dyDescent="0.3">
       <c r="G32" s="1" t="s">
@@ -1113,12 +1113,12 @@
       <c r="F41" t="s">
         <v>62</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="9"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G42" s="1" t="s">
@@ -1163,12 +1163,12 @@
       </c>
     </row>
     <row r="49" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G49" s="6" t="s">
+      <c r="G49" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="9"/>
     </row>
     <row r="50" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G50" s="1" t="s">
@@ -1213,12 +1213,12 @@
       </c>
     </row>
     <row r="56" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G56" s="6" t="s">
+      <c r="G56" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="9"/>
     </row>
     <row r="57" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G57" s="1" t="s">
@@ -1263,12 +1263,12 @@
       </c>
     </row>
     <row r="63" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G63" s="6" t="s">
+      <c r="G63" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="9"/>
     </row>
     <row r="64" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G64" s="1" t="s">
@@ -1397,12 +1397,12 @@
       </c>
     </row>
     <row r="76" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G76" s="6" t="s">
+      <c r="G76" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H76" s="7"/>
-      <c r="I76" s="7"/>
-      <c r="J76" s="8"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="9"/>
     </row>
     <row r="77" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G77" s="1" t="s">
@@ -1489,12 +1489,12 @@
       </c>
     </row>
     <row r="86" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G86" s="6" t="s">
+      <c r="G86" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H86" s="7"/>
-      <c r="I86" s="7"/>
-      <c r="J86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="9"/>
     </row>
     <row r="87" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G87" s="1" t="s">
@@ -1581,12 +1581,12 @@
       </c>
     </row>
     <row r="97" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G97" s="6" t="s">
+      <c r="G97" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H97" s="7"/>
-      <c r="I97" s="7"/>
-      <c r="J97" s="8"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="8"/>
+      <c r="J97" s="9"/>
     </row>
     <row r="98" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G98" s="1" t="s">
@@ -1659,12 +1659,12 @@
       </c>
     </row>
     <row r="105" spans="7:10" x14ac:dyDescent="0.3">
-      <c r="G105" s="6" t="s">
+      <c r="G105" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H105" s="7"/>
-      <c r="I105" s="7"/>
-      <c r="J105" s="8"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8"/>
+      <c r="J105" s="9"/>
     </row>
     <row r="106" spans="7:10" x14ac:dyDescent="0.3">
       <c r="G106" s="1" t="s">
@@ -1738,11 +1738,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G41:J41"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="H3:O6"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G8:J8"/>
     <mergeCell ref="G105:J105"/>
     <mergeCell ref="G56:J56"/>
     <mergeCell ref="G63:J63"/>
@@ -1750,6 +1745,11 @@
     <mergeCell ref="G76:J76"/>
     <mergeCell ref="G86:J86"/>
     <mergeCell ref="G97:J97"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="H3:O6"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>